<commit_message>
add tabulation 1 table
</commit_message>
<xml_diff>
--- a/utils/excelTemplate/tab1.xlsx
+++ b/utils/excelTemplate/tab1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\jr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1FBB408-4015-4B44-88E4-58023B4AF2A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED6960C4-54E1-412D-9E5B-793BFC73D2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>ตาราง ก. ตรวจสอบข้อมูลรายรับจากการขายและสินค้าคงเหลือเป็นรายไตรมาส</t>
   </si>
@@ -73,24 +73,6 @@
   </si>
   <si>
     <t>TRADEMARK</t>
-  </si>
-  <si>
-    <t>คำนำหน้านาม</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>ชื่อ</t>
-  </si>
-  <si>
-    <t>สกุล</t>
-  </si>
-  <si>
-    <t>FIRSTNAME</t>
-  </si>
-  <si>
-    <t>LASTNAME</t>
   </si>
   <si>
     <t>ปี 2567</t>
@@ -139,7 +121,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -254,6 +236,15 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -261,7 +252,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -317,10 +308,16 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="จุลภาค" xfId="1" builtinId="3"/>
-    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -625,27 +622,27 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="16" customWidth="1"/>
-    <col min="3" max="4" width="15.7109375" style="16" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" style="16" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" style="16" customWidth="1"/>
+    <col min="3" max="4" width="15.6640625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" style="16" customWidth="1"/>
+    <col min="6" max="6" width="26.33203125" style="12" customWidth="1"/>
     <col min="7" max="7" width="10" style="12" customWidth="1"/>
-    <col min="8" max="15" width="20.42578125" style="10" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="15" width="20.44140625" style="10" customWidth="1"/>
+    <col min="16" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
@@ -653,11 +650,12 @@
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
-      <c r="O2" s="15" t="s">
-        <v>20</v>
-      </c>
+      <c r="L2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="15"/>
     </row>
-    <row r="3" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="11"/>
@@ -665,95 +663,79 @@
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
     </row>
-    <row r="4" spans="1:15" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="19"/>
       <c r="J4" s="19"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="20"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="21"/>
     </row>
-    <row r="5" spans="1:15" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="D5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="E5" s="8" t="s">
         <v>6</v>
       </c>
+      <c r="F5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>9</v>
+      </c>
       <c r="I5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="K5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="O5" s="9" t="s">
+      <c r="L5" s="9" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="I4:L4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -768,7 +750,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -782,7 +764,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>